<commit_message>
Anadido confusion matrix para obtener precision de cada una de las etiquetas
</commit_message>
<xml_diff>
--- a/data/heart.xlsx
+++ b/data/heart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\ITM Prov\Proyecto Grado Ing\HearthDiseaseProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B990839-6CF0-4566-BBA0-6E191C595D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC96D8F0-3B18-46F4-9EE3-1116DAEEF5F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$2:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$M$1:$M$1027</definedName>
     <definedName name="heart" localSheetId="0">Hoja1!$A$1:$N$304</definedName>
     <definedName name="heart" localSheetId="1">Hoja2!$A$2:$N$1027</definedName>
   </definedNames>
@@ -228,9 +228,6 @@
     <t>edad</t>
   </si>
   <si>
-    <t>genero</t>
-  </si>
-  <si>
     <t>tipo de dolor pectoral</t>
   </si>
   <si>
@@ -240,28 +237,31 @@
     <t>coleterol serico</t>
   </si>
   <si>
-    <t>nivel de azucar en ayunas</t>
-  </si>
-  <si>
-    <t>resultados electrocardiograficos</t>
-  </si>
-  <si>
     <t>frecuencia cardiaca maxima</t>
-  </si>
-  <si>
-    <t>Angina Inducida Por Ejercicio</t>
   </si>
   <si>
     <t>Depresion de Onda ST</t>
   </si>
   <si>
-    <t>Pendiente del segmento</t>
+    <t>Resultado prueba  de estrés talio</t>
   </si>
   <si>
-    <t>Numero de vasos principales</t>
+    <t>genero (1:Mas, 0:Fem)</t>
   </si>
   <si>
-    <t>Resultado prueba  de estrés talio</t>
+    <t>nivel de azucar en ayunas (mayor a 120?)</t>
+  </si>
+  <si>
+    <t>Angina Inducida Por Ejercicio (1:Si, 0:No)</t>
+  </si>
+  <si>
+    <t>Pendiente del segmento ST</t>
+  </si>
+  <si>
+    <t>Numero de vasos principales (poner este numero)</t>
+  </si>
+  <si>
+    <t>resultados electrocardiograficos en reposo</t>
   </si>
 </sst>
 </file>
@@ -277,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +287,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -359,6 +371,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14040,14 +14066,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D8C928-C20F-4612-B2F6-EC58DC580B45}">
   <dimension ref="A1:O1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.28515625" style="5"/>
+    <col min="1" max="1" width="11.28515625" style="5"/>
+    <col min="2" max="2" width="12.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="5" customWidth="1"/>
@@ -14057,7 +14084,7 @@
     <col min="9" max="9" width="15.140625" style="5" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="14"/>
     <col min="11" max="11" width="14.5703125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="5" customWidth="1"/>
     <col min="13" max="13" width="17.85546875" style="5" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" style="5"/>
     <col min="15" max="15" width="11.28515625" style="3"/>
@@ -14068,31 +14095,31 @@
         <v>49</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>58</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>59</v>
@@ -14101,7 +14128,7 @@
         <v>60</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="2"/>
@@ -15471,7 +15498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>44</v>
       </c>
@@ -15515,7 +15542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>50</v>
       </c>
@@ -15559,51 +15586,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+    <row r="35" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22">
         <v>57</v>
       </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-      <c r="C35" s="5">
-        <v>0</v>
-      </c>
-      <c r="D35" s="5">
+      <c r="B35" s="22">
+        <v>1</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0</v>
+      </c>
+      <c r="D35" s="22">
         <v>130</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="22">
         <v>131</v>
       </c>
-      <c r="F35" s="5">
-        <v>0</v>
-      </c>
-      <c r="G35" s="8">
-        <v>1</v>
-      </c>
-      <c r="H35" s="5">
+      <c r="F35" s="22">
+        <v>0</v>
+      </c>
+      <c r="G35" s="23">
+        <v>1</v>
+      </c>
+      <c r="H35" s="22">
         <v>115</v>
       </c>
-      <c r="I35" s="5">
-        <v>1</v>
-      </c>
-      <c r="J35" s="14" t="s">
+      <c r="I35" s="22">
+        <v>1</v>
+      </c>
+      <c r="J35" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="5">
-        <v>1</v>
-      </c>
-      <c r="L35" s="5">
-        <v>1</v>
-      </c>
-      <c r="M35" s="5">
-        <v>3</v>
-      </c>
-      <c r="N35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K35" s="22">
+        <v>1</v>
+      </c>
+      <c r="L35" s="22">
+        <v>1</v>
+      </c>
+      <c r="M35" s="22">
+        <v>3</v>
+      </c>
+      <c r="N35" s="22">
+        <v>0</v>
+      </c>
+      <c r="O35" s="25"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>70</v>
       </c>
@@ -15647,7 +15675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>50</v>
       </c>
@@ -15691,7 +15719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>46</v>
       </c>
@@ -15735,51 +15763,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+    <row r="39" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
         <v>51</v>
       </c>
-      <c r="B39" s="5">
-        <v>1</v>
-      </c>
-      <c r="C39" s="5">
-        <v>3</v>
-      </c>
-      <c r="D39" s="5">
+      <c r="B39" s="17">
+        <v>1</v>
+      </c>
+      <c r="C39" s="17">
+        <v>3</v>
+      </c>
+      <c r="D39" s="17">
         <v>125</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="17">
         <v>213</v>
       </c>
-      <c r="F39" s="5">
-        <v>0</v>
-      </c>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
-      <c r="H39" s="5">
+      <c r="F39" s="17">
+        <v>0</v>
+      </c>
+      <c r="G39" s="18">
+        <v>0</v>
+      </c>
+      <c r="H39" s="17">
         <v>125</v>
       </c>
-      <c r="I39" s="5">
-        <v>1</v>
-      </c>
-      <c r="J39" s="14" t="s">
+      <c r="I39" s="17">
+        <v>1</v>
+      </c>
+      <c r="J39" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="K39" s="5">
-        <v>2</v>
-      </c>
-      <c r="L39" s="5">
-        <v>1</v>
-      </c>
-      <c r="M39" s="5">
-        <v>2</v>
-      </c>
-      <c r="N39" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="17">
+        <v>2</v>
+      </c>
+      <c r="L39" s="17">
+        <v>1</v>
+      </c>
+      <c r="M39" s="17">
+        <v>2</v>
+      </c>
+      <c r="N39" s="17">
+        <v>1</v>
+      </c>
+      <c r="O39" s="20"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>59</v>
       </c>
@@ -15823,7 +15852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>64</v>
       </c>
@@ -15867,7 +15896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>57</v>
       </c>
@@ -15911,7 +15940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>65</v>
       </c>
@@ -15955,7 +15984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>54</v>
       </c>
@@ -15999,7 +16028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>61</v>
       </c>
@@ -16043,7 +16072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>46</v>
       </c>
@@ -16087,7 +16116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>55</v>
       </c>
@@ -16131,7 +16160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>42</v>
       </c>
@@ -59252,7 +59281,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O2" xr:uid="{E84B51A3-52B8-49D2-B3CB-0A66914616D1}"/>
+  <autoFilter ref="M1:M1027" xr:uid="{D655B30E-B5F4-4661-90C9-65C806A92C42}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Añadidas de vuelta validaciones en el proceso de exportar a pdf. Mejorado el texto que aparece como resultado del diagnostico en el programa y en el pdf.
</commit_message>
<xml_diff>
--- a/data/heart.xlsx
+++ b/data/heart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\ITM Prov\Proyecto Grado Ing\HearthDiseaseProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC96D8F0-3B18-46F4-9EE3-1116DAEEF5F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBA7551-53DC-47F7-A3FD-831E4D837A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14066,9 +14066,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D8C928-C20F-4612-B2F6-EC58DC580B45}">
   <dimension ref="A1:O1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>